<commit_message>
Add RecordResource enhancements and CSV test files for drug imports
</commit_message>
<xml_diff>
--- a/test drugs.xlsx
+++ b/test drugs.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">emzor</t>
   </si>
   <si>
-    <t xml:space="preserve">THEATRE</t>
+    <t xml:space="preserve">ICU</t>
   </si>
   <si>
     <t xml:space="preserve">admin</t>
@@ -218,10 +218,10 @@
   <dimension ref="A1:J215"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24"/>

</xml_diff>